<commit_message>
After all fixes and flow
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="reg" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="login" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="address" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="query" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +23,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+  <si>
+    <t xml:space="preserve">Fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmpass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lovepatel1@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikk@12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himanshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">himanshi1@yopmail.com</t>
+  </si>
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -32,12 +70,6 @@
     <t xml:space="preserve">res</t>
   </si>
   <si>
-    <t xml:space="preserve">nk.gangwar581993@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nikk@12345</t>
-  </si>
-  <si>
     <t xml:space="preserve">Valid</t>
   </si>
   <si>
@@ -56,10 +88,37 @@
     <t xml:space="preserve">test123</t>
   </si>
   <si>
+    <t xml:space="preserve">company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appinventiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bareilly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noida</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
   </si>
   <si>
     <t xml:space="preserve">query</t>
@@ -381,73 +440,161 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>9411481766</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>9968198833</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16009" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -478,7 +625,100 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>242503</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>243507</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -486,7 +726,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,57 +738,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>